<commit_message>
Update modelsimv3 ingen fuktionalitet
</commit_message>
<xml_diff>
--- a/Projekt-Design-FPGA/Instuktionsæt.xlsx
+++ b/Projekt-Design-FPGA/Instuktionsæt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mozzr\Documents\GitHub\EIT4-414\Projekt-Design-FPGA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37A746A-87E4-4C05-965E-5F2F77E3CB63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0654AF85-80F2-49D1-A8B8-2973B18043D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16455" yWindow="4710" windowWidth="29145" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19035" yWindow="4785" windowWidth="19425" windowHeight="10095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="104">
   <si>
     <t>Instruktion</t>
   </si>
@@ -69,15 +69,9 @@
     <t>OP2</t>
   </si>
   <si>
-    <t>In the LT(Lesser then) case the DEST register will be 1 if OP1 is less than OP2 and 0 otherwise.</t>
-  </si>
-  <si>
     <t>EQ</t>
   </si>
   <si>
-    <t>EQ(Equal) is the same, except it checks for equality.</t>
-  </si>
-  <si>
     <t>BEQ</t>
   </si>
   <si>
@@ -225,9 +219,6 @@
     <t>Constant</t>
   </si>
   <si>
-    <t>Here DEST is the register or ram that will be set to a  CONST 8 bit value. Keep in mind that since we are making an 8 bit processor, the registers are 8 bits wide.</t>
-  </si>
-  <si>
     <t>Lesser then</t>
   </si>
   <si>
@@ -240,24 +231,12 @@
     <t>SUB OP2 from OP1 (OP1-OP2) and store the result into DEST.</t>
   </si>
   <si>
-    <t>OR, OP1 and OP2 and store their result into DEST.</t>
-  </si>
-  <si>
-    <t>AND, OP1 and OP2 and store the result into DEST.</t>
-  </si>
-  <si>
-    <t>XOR, OP1 and OP2 and store the result into DEST</t>
-  </si>
-  <si>
     <t>SHL  shift OP1 to left by OP2 bits and store the result into DEST.</t>
   </si>
   <si>
     <t>SHR  shift OP1 to right by OP2 bits and store the result into DEST.</t>
   </si>
   <si>
-    <t>JMPX Jumps back a const value (PC - (Const+1))</t>
-  </si>
-  <si>
     <t>OP</t>
   </si>
   <si>
@@ -288,15 +267,9 @@
     <t>ADDX</t>
   </si>
   <si>
-    <t>SUB, CONST from OP1 (OP1-CONST) and store the result into DEST.</t>
-  </si>
-  <si>
     <t>ADD OP1 and OP2 (OP1 + OP2) and store the result into DEST</t>
   </si>
   <si>
-    <t>ADD OP1 and a constant (OP1 + CONST) and store the result into DEST</t>
-  </si>
-  <si>
     <t>22 - 10110</t>
   </si>
   <si>
@@ -316,9 +289,6 @@
   </si>
   <si>
     <t>23 - 10111</t>
-  </si>
-  <si>
-    <t>24 - 11000</t>
   </si>
   <si>
     <t>MULT</t>
@@ -410,6 +380,39 @@
       </rPr>
       <t>21 -  10101</t>
     </r>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Here DEST is the register or ram that will be set to a  CONST 8 bit value.</t>
+  </si>
+  <si>
+    <t>DEST register will be 1 if OP1 is lesser than OP2 and 0 otherwise.</t>
+  </si>
+  <si>
+    <t>DEST register will be 1 if OP1 is equal to OP2 and 0 otherwise.</t>
+  </si>
+  <si>
+    <t>ADDX OP1 and a constant (OP1 + CONST) and store the result into DEST</t>
+  </si>
+  <si>
+    <t>SUBX CONST from OP1 (OP1-CONST) and store the result into DEST.</t>
+  </si>
+  <si>
+    <t>Logic AND of OP1 and OP2. Store the result into DEST.</t>
+  </si>
+  <si>
+    <t>Logic OR of OP1 and OP2. Store the result into DEST.</t>
+  </si>
+  <si>
+    <t>Logic XOR of OP1 and OP2. Store the result into DEST.</t>
+  </si>
+  <si>
+    <t>JMPX Jumps back a const value (PC - Const)</t>
   </si>
 </sst>
 </file>
@@ -685,7 +688,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -804,6 +807,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1092,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D5:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,24 +1125,24 @@
     <col min="15" max="15" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
+    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D5" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="24" t="s">
         <v>50</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>52</v>
       </c>
       <c r="G5" s="24" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="24" t="s">
         <v>49</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>51</v>
       </c>
       <c r="J5" s="24" t="s">
         <v>1</v>
@@ -1139,50 +1151,50 @@
         <v>3</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="18" t="s">
+      <c r="D6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="27">
-        <v>-1</v>
-      </c>
-      <c r="G6" s="27">
-        <v>-1</v>
-      </c>
-      <c r="H6" s="27">
-        <v>-1</v>
-      </c>
-      <c r="I6" s="27">
-        <v>-1</v>
-      </c>
-      <c r="J6" s="27">
-        <v>-1</v>
+      <c r="E6" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>93</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M6" s="25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="16" t="s">
+      <c r="D7" s="16" t="s">
         <v>6</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>30</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>7</v>
@@ -1190,31 +1202,31 @@
       <c r="G7" s="28">
         <v>0</v>
       </c>
-      <c r="H7" s="28">
-        <v>-1</v>
+      <c r="H7" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J7" s="28">
         <v>1</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L7" s="11" t="s">
         <v>7</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="18" t="s">
+      <c r="D8" s="18" t="s">
         <v>8</v>
+      </c>
+      <c r="E8" s="49" t="s">
+        <v>31</v>
       </c>
       <c r="F8" s="27" t="s">
         <v>7</v>
@@ -1223,68 +1235,68 @@
         <v>1</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="27">
-        <v>-1</v>
-      </c>
-      <c r="J8" s="27">
-        <v>-1</v>
+        <v>52</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>93</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L8" s="26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M8" s="26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="4:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="D9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="D9" s="16" t="s">
         <v>9</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>32</v>
       </c>
       <c r="F9" s="28" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="31">
-        <v>-1</v>
+        <v>94</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>93</v>
       </c>
       <c r="I9" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="28">
-        <v>-1</v>
+      <c r="J9" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="4:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="D10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="18" t="s">
+      <c r="D10" s="18" t="s">
         <v>11</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>33</v>
       </c>
       <c r="F10" s="27" t="s">
         <v>7</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H10" s="32" t="s">
         <v>12</v>
@@ -1293,30 +1305,30 @@
         <v>13</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="L10" s="25" t="s">
         <v>10</v>
       </c>
       <c r="M10" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="4:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="D11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>15</v>
+      <c r="D11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="50" t="s">
+        <v>34</v>
       </c>
       <c r="F11" s="28" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H11" s="31" t="s">
         <v>12</v>
@@ -1325,30 +1337,30 @@
         <v>13</v>
       </c>
       <c r="J11" s="28" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>16</v>
+        <v>97</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="4:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="D12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="27">
-        <v>-1</v>
-      </c>
-      <c r="G12" s="27">
-        <v>-1</v>
+      <c r="D12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>93</v>
       </c>
       <c r="H12" s="32" t="s">
         <v>12</v>
@@ -1356,31 +1368,31 @@
       <c r="I12" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="27">
-        <v>-1</v>
+      <c r="J12" s="27" t="s">
+        <v>93</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L12" s="25" t="s">
         <v>11</v>
       </c>
       <c r="M12" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="4:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="D13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="28">
-        <v>-1</v>
-      </c>
-      <c r="G13" s="28">
-        <v>-1</v>
+      <c r="D13" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>12</v>
@@ -1388,31 +1400,31 @@
       <c r="I13" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="28">
-        <v>-1</v>
+      <c r="J13" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="4:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="D14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>21</v>
+      <c r="D14" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>37</v>
       </c>
       <c r="F14" s="27" t="s">
         <v>7</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H14" s="32" t="s">
         <v>12</v>
@@ -1421,30 +1433,30 @@
         <v>13</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M14" s="25" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="4:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="D15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>86</v>
+      <c r="D15" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="50" t="s">
+        <v>38</v>
       </c>
       <c r="F15" s="28" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H15" s="31" t="s">
         <v>12</v>
@@ -1452,31 +1464,31 @@
       <c r="I15" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="J15" s="28">
-        <v>-1</v>
+      <c r="J15" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="4:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="D16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>22</v>
+      <c r="D16" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>39</v>
       </c>
       <c r="F16" s="27" t="s">
         <v>7</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H16" s="32" t="s">
         <v>12</v>
@@ -1485,30 +1497,30 @@
         <v>13</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L16" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M16" s="25" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="4:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="D17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>85</v>
+      <c r="D17" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="50" t="s">
+        <v>40</v>
       </c>
       <c r="F17" s="46" t="s">
         <v>7</v>
       </c>
       <c r="G17" s="42" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H17" s="45" t="s">
         <v>12</v>
@@ -1516,31 +1528,31 @@
       <c r="I17" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="J17" s="46">
-        <v>-1</v>
+      <c r="J17" s="46" t="s">
+        <v>93</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>98</v>
+      <c r="D18" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>41</v>
       </c>
       <c r="F18" s="19" t="s">
         <v>7</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H18" s="20" t="s">
         <v>12</v>
@@ -1549,30 +1561,30 @@
         <v>13</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="L18" s="25" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="M18" s="25" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="44" t="s">
-        <v>93</v>
+      <c r="D19" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="50" t="s">
+        <v>42</v>
       </c>
       <c r="F19" s="21" t="s">
         <v>7</v>
       </c>
       <c r="G19" s="43" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H19" s="34" t="s">
         <v>12</v>
@@ -1581,24 +1593,24 @@
         <v>13</v>
       </c>
       <c r="J19" s="21" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>23</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="D20" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>43</v>
       </c>
       <c r="F20" s="27" t="s">
         <v>7</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H20" s="32" t="s">
         <v>12</v>
@@ -1607,24 +1619,24 @@
         <v>13</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>24</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="D21" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="50" t="s">
+        <v>44</v>
       </c>
       <c r="F21" s="28" t="s">
         <v>7</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H21" s="28" t="s">
         <v>12</v>
@@ -1633,50 +1645,50 @@
         <v>13</v>
       </c>
       <c r="J21" s="28" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="4:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="D22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>25</v>
+      <c r="D22" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>45</v>
       </c>
       <c r="F22" s="27" t="s">
         <v>7</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="27">
-        <v>-1</v>
+        <v>94</v>
+      </c>
+      <c r="H22" s="27" t="s">
+        <v>93</v>
       </c>
       <c r="I22" s="27" t="s">
         <v>12</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D23" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="D23" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="51" t="s">
+        <v>46</v>
       </c>
       <c r="F23" s="28" t="s">
         <v>7</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H23" s="28" t="s">
         <v>12</v>
@@ -1685,68 +1697,66 @@
         <v>13</v>
       </c>
       <c r="J23" s="28" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D24" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="F24" s="29">
-        <v>-1</v>
-      </c>
-      <c r="G24" s="29">
-        <v>-1</v>
-      </c>
-      <c r="H24" s="30">
-        <v>-1</v>
+      <c r="D24" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="I24" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="J24" s="29">
-        <v>-1</v>
+      <c r="J24" s="29" t="s">
+        <v>93</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D25" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E25" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" s="28">
-        <v>-1</v>
-      </c>
-      <c r="G25" s="28">
-        <v>-1</v>
-      </c>
-      <c r="H25" s="31">
-        <v>-1</v>
+      <c r="D25" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="H25" s="31" t="s">
+        <v>93</v>
       </c>
       <c r="I25" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="J25" s="28">
-        <v>-1</v>
+      <c r="J25" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D26" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="37"/>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
@@ -1756,9 +1766,7 @@
       <c r="K26" s="14"/>
     </row>
     <row r="27" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D27" s="3">
-        <v>25</v>
-      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="38"/>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -1768,9 +1776,7 @@
       <c r="K27" s="8"/>
     </row>
     <row r="28" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D28" s="2">
-        <v>26</v>
-      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="37"/>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
@@ -1780,9 +1786,7 @@
       <c r="K28" s="14"/>
     </row>
     <row r="29" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D29" s="3">
-        <v>27</v>
-      </c>
+      <c r="D29" s="3"/>
       <c r="E29" s="38"/>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -1792,9 +1796,7 @@
       <c r="K29" s="8"/>
     </row>
     <row r="30" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D30" s="2">
-        <v>28</v>
-      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="37"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
@@ -1804,9 +1806,7 @@
       <c r="K30" s="14"/>
     </row>
     <row r="31" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D31" s="3">
-        <v>29</v>
-      </c>
+      <c r="D31" s="3"/>
       <c r="E31" s="38"/>
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
@@ -1816,9 +1816,7 @@
       <c r="K31" s="8"/>
     </row>
     <row r="32" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D32" s="2">
-        <v>30</v>
-      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="37"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
@@ -1828,9 +1826,7 @@
       <c r="K32" s="14"/>
     </row>
     <row r="33" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D33" s="3">
-        <v>31</v>
-      </c>
+      <c r="D33" s="3"/>
       <c r="E33" s="38"/>
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
@@ -1840,9 +1836,7 @@
       <c r="K33" s="8"/>
     </row>
     <row r="34" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D34" s="2">
-        <v>32</v>
-      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="37"/>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
@@ -1852,9 +1846,7 @@
       <c r="K34" s="14"/>
     </row>
     <row r="35" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D35" s="3">
-        <v>33</v>
-      </c>
+      <c r="D35" s="3"/>
       <c r="E35" s="38"/>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
@@ -1864,9 +1856,7 @@
       <c r="K35" s="8"/>
     </row>
     <row r="36" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D36" s="9">
-        <v>34</v>
-      </c>
+      <c r="D36" s="9"/>
       <c r="E36" s="39"/>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
@@ -1877,19 +1867,19 @@
     </row>
     <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="47" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F44" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G44" s="29">
         <v>1</v>
       </c>
       <c r="H44" s="30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I44" s="29">
         <v>-1</v>
@@ -1898,15 +1888,15 @@
         <v>-1</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="47" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F46" s="29" t="s">
         <v>7</v>
@@ -1915,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="H46" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I46" s="29">
         <v>-1</v>
@@ -1924,21 +1914,21 @@
         <v>-1</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="4:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D48" s="47" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E48" s="40" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F48" s="27" t="s">
         <v>7</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H48" s="41" t="s">
         <v>12</v>
@@ -1947,24 +1937,24 @@
         <v>13</v>
       </c>
       <c r="J48" s="27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="4:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D49" s="48" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F49" s="28" t="s">
         <v>7</v>
       </c>
       <c r="G49" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H49" s="28" t="s">
         <v>12</v>
@@ -1973,10 +1963,10 @@
         <v>13</v>
       </c>
       <c r="J49" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tilføjet assemblersyntax til instrukssæt
</commit_message>
<xml_diff>
--- a/Projekt-Design-FPGA/Instuktionsæt.xlsx
+++ b/Projekt-Design-FPGA/Instuktionsæt.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mozzr\Documents\GitHub\EIT4-414\Projekt-Design-FPGA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marie\Documents\GitHub\EIT4-414\Projekt-Design-FPGA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0654AF85-80F2-49D1-A8B8-2973B18043D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19035" yWindow="4785" windowWidth="19425" windowHeight="10095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19035" yWindow="4785" windowWidth="19425" windowHeight="10095"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="109">
   <si>
     <t>Instruktion</t>
   </si>
@@ -414,11 +413,26 @@
   <si>
     <t>JMPX Jumps back a const value (PC - Const)</t>
   </si>
+  <si>
+    <t>LOAD #1 #2</t>
+  </si>
+  <si>
+    <t>STORE #1 #2</t>
+  </si>
+  <si>
+    <t>SET #1 MEM #3</t>
+  </si>
+  <si>
+    <t>LT #1 MEM #2 #3 MEM</t>
+  </si>
+  <si>
+    <t>Assembler-form</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -819,11 +833,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="20 % - Farve2" xfId="5" builtinId="34"/>
-    <cellStyle name="20 % - Farve3" xfId="1" builtinId="38"/>
-    <cellStyle name="20 % - Farve4" xfId="2" builtinId="42"/>
-    <cellStyle name="20 % - Farve5" xfId="3" builtinId="46"/>
-    <cellStyle name="Beregning" xfId="4" builtinId="22"/>
+    <cellStyle name="20% - Accent2" xfId="5" builtinId="34"/>
+    <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
+    <cellStyle name="20% - Accent4" xfId="2" builtinId="42"/>
+    <cellStyle name="20% - Accent5" xfId="3" builtinId="46"/>
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1101,16 +1115,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D5:M49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="3" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
@@ -1125,7 +1141,10 @@
     <col min="15" max="15" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
       <c r="D5" s="23" t="s">
         <v>0</v>
       </c>
@@ -1157,7 +1176,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
       <c r="D6" s="18" t="s">
         <v>4</v>
       </c>
@@ -1189,7 +1211,10 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>104</v>
+      </c>
       <c r="D7" s="16" t="s">
         <v>6</v>
       </c>
@@ -1221,7 +1246,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>105</v>
+      </c>
       <c r="D8" s="18" t="s">
         <v>8</v>
       </c>
@@ -1253,7 +1281,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>106</v>
+      </c>
       <c r="D9" s="16" t="s">
         <v>9</v>
       </c>
@@ -1285,7 +1316,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>107</v>
+      </c>
       <c r="D10" s="18" t="s">
         <v>11</v>
       </c>
@@ -1317,7 +1351,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="4:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:13" ht="45" x14ac:dyDescent="0.25">
       <c r="D11" s="16" t="s">
         <v>14</v>
       </c>
@@ -1349,7 +1383,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="4:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:13" ht="60" x14ac:dyDescent="0.25">
       <c r="D12" s="18" t="s">
         <v>15</v>
       </c>
@@ -1381,7 +1415,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:13" ht="30" x14ac:dyDescent="0.25">
       <c r="D13" s="16" t="s">
         <v>17</v>
       </c>
@@ -1413,7 +1447,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:13" ht="30" x14ac:dyDescent="0.25">
       <c r="D14" s="18" t="s">
         <v>19</v>
       </c>
@@ -1445,7 +1479,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:13" ht="30" x14ac:dyDescent="0.25">
       <c r="D15" s="16" t="s">
         <v>79</v>
       </c>
@@ -1477,7 +1511,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:13" ht="30" x14ac:dyDescent="0.25">
       <c r="D16" s="18" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
flettet fungerer med" 24+7, vis og reset"
</commit_message>
<xml_diff>
--- a/Projekt-Design-FPGA/Instuktionsæt.xlsx
+++ b/Projekt-Design-FPGA/Instuktionsæt.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="117">
   <si>
     <t>Instruktion</t>
   </si>
@@ -427,6 +427,30 @@
   </si>
   <si>
     <t>Assembler-form</t>
+  </si>
+  <si>
+    <t>VAL1</t>
+  </si>
+  <si>
+    <t>VAL2</t>
+  </si>
+  <si>
+    <t>ANS</t>
+  </si>
+  <si>
+    <t>AJ</t>
+  </si>
+  <si>
+    <t>27 - 11011</t>
+  </si>
+  <si>
+    <t>26 - 11010</t>
+  </si>
+  <si>
+    <t>25 - 11001</t>
+  </si>
+  <si>
+    <t>24 - 11000</t>
   </si>
 </sst>
 </file>
@@ -702,7 +726,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -830,6 +854,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1116,10 +1153,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:M49"/>
+  <dimension ref="C5:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,43 +1837,99 @@
       <c r="K26" s="14"/>
     </row>
     <row r="27" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D27" s="3"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
+      <c r="D27" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="46">
+        <v>0</v>
+      </c>
+      <c r="H27" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="I27" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="J27" s="52" t="s">
+        <v>93</v>
+      </c>
       <c r="K27" s="8"/>
     </row>
     <row r="28" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D28" s="2"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="D28" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="29">
+        <v>0</v>
+      </c>
+      <c r="H28" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="I28" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="J28" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="K28" s="14"/>
     </row>
     <row r="29" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D29" s="3"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
+      <c r="D29" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="G29" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="H29" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="I29" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="J29" s="52" t="s">
+        <v>93</v>
+      </c>
       <c r="K29" s="8"/>
     </row>
     <row r="30" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D30" s="2"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
+      <c r="D30" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="29">
+        <v>0</v>
+      </c>
+      <c r="H30" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="I30" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="J30" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="K30" s="14"/>
     </row>
     <row r="31" spans="4:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
IO kerne / Flet2 update
</commit_message>
<xml_diff>
--- a/Projekt-Design-FPGA/Instuktionsæt.xlsx
+++ b/Projekt-Design-FPGA/Instuktionsæt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mozzr\Documents\GitHub\EIT4-414\Projekt-Design-FPGA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1117DD-5CF0-467A-9403-2D3BAE38CEF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425C7555-D83C-4679-8BFE-2B62C6D4431A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="136">
   <si>
     <t>Instruktion</t>
   </si>
@@ -506,6 +506,9 @@
   </si>
   <si>
     <t>BNEQ src(reg) val</t>
+  </si>
+  <si>
+    <t>TBR</t>
   </si>
 </sst>
 </file>
@@ -1213,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,13 +2048,27 @@
       <c r="K30" s="14"/>
     </row>
     <row r="31" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="D31" s="3"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
+      <c r="D31" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="I31" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="J31" s="21" t="s">
+        <v>92</v>
+      </c>
       <c r="K31" s="8"/>
     </row>
     <row r="32" spans="3:13" x14ac:dyDescent="0.25">

</xml_diff>